<commit_message>
função para definição de épocas
</commit_message>
<xml_diff>
--- a/output/estat-desc.xlsx
+++ b/output/estat-desc.xlsx
@@ -397,7 +397,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>dry_2015</t>
+          <t>dry_15:16</t>
         </is>
       </c>
       <c r="B2">
@@ -422,7 +422,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>dry_2016</t>
+          <t>dry_16:17</t>
         </is>
       </c>
       <c r="B3">
@@ -447,7 +447,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>dry_2017</t>
+          <t>dry_17:18</t>
         </is>
       </c>
       <c r="B4">
@@ -472,7 +472,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>dry_2018</t>
+          <t>dry_18:19</t>
         </is>
       </c>
       <c r="B5">
@@ -497,7 +497,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>dry_2019</t>
+          <t>dry_19:20</t>
         </is>
       </c>
       <c r="B6">
@@ -522,7 +522,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>dry_2020</t>
+          <t>dry_20:21</t>
         </is>
       </c>
       <c r="B7">
@@ -547,7 +547,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>dry_2021</t>
+          <t>dry_21:22</t>
         </is>
       </c>
       <c r="B8">
@@ -572,7 +572,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>dry_2022</t>
+          <t>dry_22:23</t>
         </is>
       </c>
       <c r="B9">
@@ -597,7 +597,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>dry_2023</t>
+          <t>dry_23:24</t>
         </is>
       </c>
       <c r="B10">
@@ -622,7 +622,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>rainy_2015-2016</t>
+          <t>rainy_15:16</t>
         </is>
       </c>
       <c r="B11">
@@ -647,7 +647,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>rainy_2016-2017</t>
+          <t>rainy_16:17</t>
         </is>
       </c>
       <c r="B12">
@@ -672,7 +672,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>rainy_2017-2018</t>
+          <t>rainy_17:18</t>
         </is>
       </c>
       <c r="B13">
@@ -697,7 +697,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>rainy_2018-2019</t>
+          <t>rainy_18:19</t>
         </is>
       </c>
       <c r="B14">
@@ -722,7 +722,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>rainy_2019-2020</t>
+          <t>rainy_19:20</t>
         </is>
       </c>
       <c r="B15">
@@ -747,7 +747,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>rainy_2020-2021</t>
+          <t>rainy_20:21</t>
         </is>
       </c>
       <c r="B16">
@@ -772,7 +772,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>rainy_2021-2022</t>
+          <t>rainy_21:22</t>
         </is>
       </c>
       <c r="B17">
@@ -797,7 +797,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>rainy_2022-2023</t>
+          <t>rainy_22:23</t>
         </is>
       </c>
       <c r="B18">
@@ -822,7 +822,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>rainy_2023-2024</t>
+          <t>rainy_23:24</t>
         </is>
       </c>
       <c r="B19">

</xml_diff>

<commit_message>
anomalia e centro de massa
</commit_message>
<xml_diff>
--- a/output/estat-desc.xlsx
+++ b/output/estat-desc.xlsx
@@ -404,10 +404,10 @@
         <v>3170</v>
       </c>
       <c r="C2">
-        <v>388.1002812414737</v>
+        <v>387.1016018289494</v>
       </c>
       <c r="D2">
-        <v>388.125496375959</v>
+        <v>387.1268169634347</v>
       </c>
       <c r="E2">
         <v>1.18230522900363</v>
@@ -429,10 +429,10 @@
         <v>3072</v>
       </c>
       <c r="C3">
-        <v>388.6085888272675</v>
+        <v>387.5687990774547</v>
       </c>
       <c r="D3">
-        <v>388.6315248435886</v>
+        <v>387.5917350937759</v>
       </c>
       <c r="E3">
         <v>1.536246302957206</v>
@@ -454,10 +454,10 @@
         <v>2256</v>
       </c>
       <c r="C4">
-        <v>388.2635566983448</v>
+        <v>387.1826566112436</v>
       </c>
       <c r="D4">
-        <v>388.3199568756714</v>
+        <v>387.2390567885702</v>
       </c>
       <c r="E4">
         <v>1.215865786736222</v>
@@ -479,10 +479,10 @@
         <v>2715</v>
       </c>
       <c r="C5">
-        <v>388.0634984551813</v>
+        <v>386.9414880307917</v>
       </c>
       <c r="D5">
-        <v>388.1058773110745</v>
+        <v>386.9838668866848</v>
       </c>
       <c r="E5">
         <v>1.625165666039994</v>
@@ -504,10 +504,10 @@
         <v>2718</v>
       </c>
       <c r="C6">
-        <v>388.4256258081519</v>
+        <v>387.2625050464738</v>
       </c>
       <c r="D6">
-        <v>388.5321480882745</v>
+        <v>387.3690273265964</v>
       </c>
       <c r="E6">
         <v>1.392900313456778</v>
@@ -529,10 +529,10 @@
         <v>2629</v>
       </c>
       <c r="C7">
-        <v>388.0215566120481</v>
+        <v>386.8173255130815</v>
       </c>
       <c r="D7">
-        <v>388.100661297115</v>
+        <v>386.8964301981485</v>
       </c>
       <c r="E7">
         <v>1.752316074368826</v>
@@ -554,10 +554,10 @@
         <v>2809</v>
       </c>
       <c r="C8">
-        <v>388.684828719828</v>
+        <v>387.439487283573</v>
       </c>
       <c r="D8">
-        <v>388.8488620059557</v>
+        <v>387.6035205697006</v>
       </c>
       <c r="E8">
         <v>1.539506506405061</v>
@@ -579,10 +579,10 @@
         <v>1215</v>
       </c>
       <c r="C9">
-        <v>388.7252691201219</v>
+        <v>387.4388173465784</v>
       </c>
       <c r="D9">
-        <v>388.8230453808118</v>
+        <v>387.5365936072684</v>
       </c>
       <c r="E9">
         <v>1.620785703530477</v>
@@ -604,10 +604,10 @@
         <v>1937</v>
       </c>
       <c r="C10">
-        <v>388.2969981801617</v>
+        <v>386.9694360693297</v>
       </c>
       <c r="D10">
-        <v>388.3163632771524</v>
+        <v>386.9888011663205</v>
       </c>
       <c r="E10">
         <v>1.506517856368988</v>
@@ -629,19 +629,19 @@
         <v>1838</v>
       </c>
       <c r="C11">
-        <v>388.1957645963454</v>
+        <v>387.1909790238212</v>
       </c>
       <c r="D11">
-        <v>388.3089833144356</v>
+        <v>387.3076946489816</v>
       </c>
       <c r="E11">
-        <v>1.184910438009825</v>
+        <v>1.192266613200502</v>
       </c>
       <c r="F11">
-        <v>-0.6798958868693163</v>
+        <v>-0.6937070539837423</v>
       </c>
       <c r="G11">
-        <v>1.37780710172395</v>
+        <v>1.380739891101147</v>
       </c>
     </row>
     <row r="12">
@@ -654,19 +654,19 @@
         <v>1885</v>
       </c>
       <c r="C12">
-        <v>388.5742378695879</v>
+        <v>387.5317655884826</v>
       </c>
       <c r="D12">
-        <v>388.6906831687839</v>
+        <v>387.6479332138931</v>
       </c>
       <c r="E12">
-        <v>1.329770677972302</v>
+        <v>1.333573253186748</v>
       </c>
       <c r="F12">
-        <v>-0.2363495003273333</v>
+        <v>-0.2459064695264767</v>
       </c>
       <c r="G12">
-        <v>0.2284416115427801</v>
+        <v>0.2357726206422357</v>
       </c>
     </row>
     <row r="13">
@@ -679,19 +679,19 @@
         <v>1167</v>
       </c>
       <c r="C13">
-        <v>388.4313482405082</v>
+        <v>387.345868595697</v>
       </c>
       <c r="D13">
-        <v>388.4990035065308</v>
+        <v>387.4181034194296</v>
       </c>
       <c r="E13">
-        <v>1.456608406129443</v>
+        <v>1.463258557030148</v>
       </c>
       <c r="F13">
-        <v>-0.4428908189928156</v>
+        <v>-0.4569013605566123</v>
       </c>
       <c r="G13">
-        <v>0.9626118266681516</v>
+        <v>0.9812587943120659</v>
       </c>
     </row>
     <row r="14">
@@ -704,19 +704,19 @@
         <v>1332</v>
       </c>
       <c r="C14">
-        <v>388.2689046757055</v>
+        <v>387.1412462094812</v>
       </c>
       <c r="D14">
-        <v>388.3415645669339</v>
+        <v>387.217081261914</v>
       </c>
       <c r="E14">
-        <v>1.42492878387142</v>
+        <v>1.432882181232127</v>
       </c>
       <c r="F14">
-        <v>-0.4222469525211169</v>
+        <v>-0.4359629151490947</v>
       </c>
       <c r="G14">
-        <v>0.7451067570683718</v>
+        <v>0.7483782737744353</v>
       </c>
     </row>
     <row r="15">
@@ -729,19 +729,19 @@
         <v>1477</v>
       </c>
       <c r="C15">
-        <v>389.6029235043545</v>
+        <v>388.4381883895534</v>
       </c>
       <c r="D15">
-        <v>389.6434762132745</v>
+        <v>388.4803554515964</v>
       </c>
       <c r="E15">
-        <v>1.441839574703427</v>
+        <v>1.445688955703633</v>
       </c>
       <c r="F15">
-        <v>-0.5635163100621993</v>
+        <v>-0.5779276682639747</v>
       </c>
       <c r="G15">
-        <v>2.077076396052272</v>
+        <v>2.11375978505539</v>
       </c>
     </row>
     <row r="16">
@@ -754,19 +754,19 @@
         <v>856</v>
       </c>
       <c r="C16">
-        <v>389.6187140743696</v>
+        <v>388.4124658794146</v>
       </c>
       <c r="D16">
-        <v>389.6833028986775</v>
+        <v>388.479071799711</v>
       </c>
       <c r="E16">
-        <v>1.584106363923727</v>
+        <v>1.587305773226825</v>
       </c>
       <c r="F16">
-        <v>-0.1515436040132707</v>
+        <v>-0.1581859639359714</v>
       </c>
       <c r="G16">
-        <v>0.1141165969337377</v>
+        <v>0.1198330976075468</v>
       </c>
     </row>
     <row r="17">
@@ -779,19 +779,19 @@
         <v>1445</v>
       </c>
       <c r="C17">
-        <v>389.0115019627246</v>
+        <v>387.7634293206705</v>
       </c>
       <c r="D17">
-        <v>388.9236911075182</v>
+        <v>387.6771289681381</v>
       </c>
       <c r="E17">
-        <v>1.690878643781657</v>
+        <v>1.69418452977483</v>
       </c>
       <c r="F17">
-        <v>0.4007713550468281</v>
+        <v>0.3939887492320298</v>
       </c>
       <c r="G17">
-        <v>0.1522522362822292</v>
+        <v>0.152294289086699</v>
       </c>
     </row>
     <row r="18">
@@ -804,19 +804,19 @@
         <v>1747</v>
       </c>
       <c r="C18">
-        <v>388.4184057729926</v>
+        <v>387.1302126342749</v>
       </c>
       <c r="D18">
-        <v>388.458085664015</v>
+        <v>387.1716338904715</v>
       </c>
       <c r="E18">
-        <v>1.347290108531668</v>
+        <v>1.351063952638233</v>
       </c>
       <c r="F18">
-        <v>-0.1042603627205105</v>
+        <v>-0.1214769430852471</v>
       </c>
       <c r="G18">
-        <v>2.063800425412113</v>
+        <v>2.089503294318475</v>
       </c>
     </row>
     <row r="19">
@@ -829,10 +829,10 @@
         <v>1408</v>
       </c>
       <c r="C19">
-        <v>389.260462551701</v>
+        <v>387.9329004408691</v>
       </c>
       <c r="D19">
-        <v>389.1278714558634</v>
+        <v>387.8003093450315</v>
       </c>
       <c r="E19">
         <v>1.338840305557669</v>

</xml_diff>